<commit_message>
Changes in orc-vcr model
</commit_message>
<xml_diff>
--- a/Examples/orcvcr/orcvcr_model.xlsx
+++ b/Examples/orcvcr/orcvcr_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Termoeconomia\TaesLab\Examples\orcvcr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\orcvcr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59F6B79-4472-4CF2-B418-662680B81384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCD9BA7-03F6-4512-A6B7-541B192FDB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="375" windowWidth="17265" windowHeight="12525" firstSheet="3" activeTab="5" xr2:uid="{E29BBF69-888A-4B0D-A36F-5F6BD99DC033}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="23550" windowHeight="13635" activeTab="4" xr2:uid="{E29BBF69-888A-4B0D-A36F-5F6BD99DC033}"/>
   </bookViews>
   <sheets>
     <sheet name="Physical Diagram" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,7 @@
     <sheet name="Exergy" sheetId="6" r:id="rId5"/>
     <sheet name="Format" sheetId="5" r:id="rId6"/>
     <sheet name="WasteDefinition" sheetId="7" r:id="rId7"/>
-    <sheet name="WasteAllocation" sheetId="8" r:id="rId8"/>
-    <sheet name="ResourcesCost" sheetId="9" r:id="rId9"/>
+    <sheet name="ResourcesCost" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="DATOS" localSheetId="4">Exergy!#REF!</definedName>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="86">
   <si>
     <t>Flows</t>
   </si>
@@ -284,15 +283,6 @@
     <t>DIAGNOSIS</t>
   </si>
   <si>
-    <t>R134a</t>
-  </si>
-  <si>
-    <t>R1234ze</t>
-  </si>
-  <si>
-    <t>R227ea</t>
-  </si>
-  <si>
     <t>recycle</t>
   </si>
   <si>
@@ -314,9 +304,6 @@
     <t>REF</t>
   </si>
   <si>
-    <t>WT10</t>
-  </si>
-  <si>
     <t>External</t>
   </si>
   <si>
@@ -324,6 +311,15 @@
   </si>
   <si>
     <t>(c$/kWh)</t>
+  </si>
+  <si>
+    <t>ETAC75</t>
+  </si>
+  <si>
+    <t>TCND35</t>
+  </si>
+  <si>
+    <t>TBLR85</t>
   </si>
 </sst>
 </file>
@@ -345,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +360,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -383,11 +373,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,7 +1004,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -1192,7 +1181,7 @@
         <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -1234,430 +1223,360 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C71C192-3DC3-406B-9DFF-73A67AE08F6E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>Flows!A2</f>
-        <v>B1</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>85.15</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="C2">
-        <v>112.7</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="D2">
-        <v>91.23</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="E2">
-        <v>128.6</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="F2">
-        <v>108.6</v>
-      </c>
-      <c r="G2">
-        <v>105.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>Flows!A3</f>
-        <v>B2</v>
+        <v>129.69999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>43.6</v>
+        <v>68.78</v>
       </c>
       <c r="C3">
-        <v>57.7</v>
+        <v>69</v>
       </c>
       <c r="D3">
-        <v>46.86</v>
+        <v>68.78</v>
       </c>
       <c r="E3">
-        <v>83.15</v>
+        <v>75.55</v>
       </c>
       <c r="F3">
-        <v>61.96</v>
-      </c>
-      <c r="G3">
-        <v>61.87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>Flows!A4</f>
-        <v>B3</v>
+        <v>68.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
       </c>
       <c r="B4">
-        <v>38.630000000000003</v>
+        <v>60.94</v>
       </c>
       <c r="C4">
-        <v>51.13</v>
+        <v>60.94</v>
       </c>
       <c r="D4">
-        <v>41.39</v>
+        <v>60.94</v>
       </c>
       <c r="E4">
-        <v>78.25</v>
+        <v>61.44</v>
       </c>
       <c r="F4">
-        <v>55.76</v>
-      </c>
-      <c r="G4">
-        <v>57.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>Flows!A5</f>
-        <v>B4</v>
+        <v>60.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>40.36</v>
+        <v>63.68</v>
       </c>
       <c r="C5">
-        <v>53.42</v>
+        <v>63.68</v>
       </c>
       <c r="D5">
-        <v>43.24</v>
+        <v>63.68</v>
       </c>
       <c r="E5">
-        <v>82.03</v>
+        <v>64.08</v>
       </c>
       <c r="F5">
-        <v>59.33</v>
-      </c>
-      <c r="G5">
-        <v>59.89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>Flows!A6</f>
-        <v>B5</v>
+        <v>63.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>43.79</v>
+        <v>37.97</v>
       </c>
       <c r="C6">
-        <v>43.79</v>
+        <v>34.79</v>
       </c>
       <c r="D6">
-        <v>43.79</v>
+        <v>37.979999999999997</v>
       </c>
       <c r="E6">
-        <v>67.66</v>
+        <v>30.41</v>
       </c>
       <c r="F6">
-        <v>55.39</v>
-      </c>
-      <c r="G6">
-        <v>56.31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>Flows!A7</f>
-        <v>B6</v>
+        <v>34.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>41.06</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="C7">
-        <v>41.06</v>
+        <v>30.58</v>
       </c>
       <c r="D7">
-        <v>41.06</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="E7">
-        <v>64.61</v>
+        <v>25.68</v>
       </c>
       <c r="F7">
-        <v>51.27</v>
-      </c>
-      <c r="G7">
-        <v>53.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>Flows!A8</f>
-        <v>B7</v>
+        <v>30.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
       </c>
       <c r="B8">
-        <v>23.09</v>
+        <v>10.25</v>
       </c>
       <c r="C8">
-        <v>23.09</v>
+        <v>9.3889999999999993</v>
       </c>
       <c r="D8">
-        <v>23.09</v>
+        <v>10.25</v>
       </c>
       <c r="E8">
-        <v>46.65</v>
+        <v>8.1389999999999993</v>
       </c>
       <c r="F8">
-        <v>33.450000000000003</v>
-      </c>
-      <c r="G8">
-        <v>35.380000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>Flows!A9</f>
-        <v>B8</v>
+        <v>9.3989999999999991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
       </c>
       <c r="B9">
-        <v>48.44</v>
+        <v>42.06</v>
       </c>
       <c r="C9">
-        <v>48.44</v>
+        <v>38.53</v>
       </c>
       <c r="D9">
-        <v>48.44</v>
+        <v>42.09</v>
       </c>
       <c r="E9">
-        <v>72.45</v>
+        <v>36.65</v>
       </c>
       <c r="F9">
-        <v>60.3</v>
-      </c>
-      <c r="G9">
-        <v>61.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>Flows!A10</f>
-        <v>WT</v>
+        <v>38.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
       </c>
       <c r="B10">
-        <v>33.619999999999997</v>
+        <v>53.04</v>
       </c>
       <c r="C10">
-        <v>44.5</v>
+        <v>49.72</v>
       </c>
       <c r="D10">
-        <v>33.770000000000003</v>
+        <v>53.04</v>
       </c>
       <c r="E10">
-        <v>36.51</v>
+        <v>47.67</v>
       </c>
       <c r="F10">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="G10">
+        <v>49.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>39.57</v>
+      </c>
+      <c r="C11">
+        <v>36.25</v>
+      </c>
+      <c r="D11">
+        <v>40.590000000000003</v>
+      </c>
+      <c r="E11">
         <v>35.340000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>Flows!A11</f>
-        <v>WC</v>
-      </c>
-      <c r="B11">
-        <v>31.55</v>
-      </c>
-      <c r="C11">
-        <v>31.55</v>
-      </c>
-      <c r="D11">
-        <v>31.55</v>
-      </c>
-      <c r="E11">
+      <c r="F11">
+        <v>36.29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="C12">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="D12">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="E12">
+        <v>3.0859999999999999</v>
+      </c>
+      <c r="F12">
+        <v>2.8039999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>104.9</v>
+      </c>
+      <c r="C13">
+        <v>104.9</v>
+      </c>
+      <c r="D13">
+        <v>104.9</v>
+      </c>
+      <c r="E13">
+        <v>101.6</v>
+      </c>
+      <c r="F13">
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="F11">
-        <v>33.42</v>
-      </c>
-      <c r="G11">
-        <v>31.91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>Flows!A12</f>
-        <v>WP</v>
-      </c>
-      <c r="B12">
-        <v>2.0310000000000001</v>
-      </c>
-      <c r="C12">
-        <v>2.6880000000000002</v>
-      </c>
-      <c r="D12">
-        <v>2.1760000000000002</v>
-      </c>
-      <c r="E12">
-        <v>4.4210000000000003</v>
-      </c>
-      <c r="F12">
-        <v>4.1879999999999997</v>
-      </c>
-      <c r="G12">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>Flows!A13</f>
-        <v>QBLR</v>
-      </c>
-      <c r="B13">
-        <v>63.42</v>
-      </c>
-      <c r="C13">
-        <v>83.94</v>
-      </c>
-      <c r="D13">
-        <v>67.95</v>
-      </c>
-      <c r="E13">
-        <v>69.33</v>
-      </c>
-      <c r="F13">
-        <v>75.849999999999994</v>
-      </c>
-      <c r="G13">
-        <v>67.709999999999994</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>Flows!A14</f>
-        <v>QEVP</v>
-      </c>
       <c r="B14">
-        <v>13.24</v>
+        <v>18.920000000000002</v>
       </c>
       <c r="C14">
-        <v>13.24</v>
+        <v>17.34</v>
       </c>
       <c r="D14">
-        <v>13.24</v>
+        <v>18.920000000000002</v>
       </c>
       <c r="E14">
-        <v>13.24</v>
+        <v>14.35</v>
       </c>
       <c r="F14">
-        <v>13.24</v>
-      </c>
-      <c r="G14">
-        <v>13.24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>Flows!A15</f>
-        <v>WN</v>
+        <v>17.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>Flows!A16</f>
-        <v>QEXP</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
       </c>
       <c r="B16">
-        <f>B6-B7</f>
-        <v>2.7299999999999969</v>
+        <f>Exergy!B6-Exergy!B7</f>
+        <v>4.5899999999999963</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:G16" si="0">C6-C7</f>
-        <v>2.7299999999999969</v>
+        <f>Exergy!C6-Exergy!C7</f>
+        <v>4.2100000000000009</v>
       </c>
       <c r="D16">
+        <v>4.5949999999999998</v>
+      </c>
+      <c r="E16">
+        <f>Exergy!E6-Exergy!E7</f>
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="F16">
+        <f>Exergy!F6-Exergy!F7</f>
+        <v>4.2100000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:F17" si="0">B3-B4+B9-B6</f>
+        <v>11.930000000000007</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>2.7299999999999969</v>
-      </c>
-      <c r="E16">
+        <v>11.800000000000004</v>
+      </c>
+      <c r="D17">
+        <v>11.95</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="0"/>
-        <v>3.0499999999999972</v>
-      </c>
-      <c r="F16">
+        <v>20.349999999999998</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="0"/>
-        <v>4.1199999999999974</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>3.1400000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>Flows!A17</f>
-        <v>QCND</v>
-      </c>
-      <c r="B17">
-        <f t="shared" ref="B17:C17" si="1">B3-B4+B9-B6</f>
-        <v>9.6199999999999974</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>11.219999999999999</v>
-      </c>
-      <c r="D17">
-        <v>10.119999999999999</v>
-      </c>
-      <c r="E17">
-        <f>E3-E4+E9-E6</f>
-        <v>9.6900000000000119</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ref="F17:G17" si="2">F3-F4+F9-F6</f>
-        <v>11.11</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
-        <v>9.5600000000000023</v>
+        <v>11.430000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -1669,7 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0C34D9-3156-4D42-9D3A-CA3AAFB07BAA}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1703,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,7 +1678,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,7 +1692,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1802,15 +1721,15 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1845,98 +1764,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5F385F-C817-40BD-A5CF-BFEFDFAA0650}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C739F77A-4BB8-47BE-8329-5157E8DF3B0D}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1951,13 +1778,13 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>